<commit_message>
Review data on methane
</commit_message>
<xml_diff>
--- a/methane/data/methane_data.xlsx
+++ b/methane/data/methane_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15990" windowHeight="8370" tabRatio="719" activeTab="2"/>
+    <workbookView windowWidth="15990" windowHeight="9405" tabRatio="719" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CCmd" sheetId="1" r:id="rId1"/>
@@ -143,10 +143,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -160,15 +160,30 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -180,17 +195,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -211,22 +220,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,58 +238,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -307,6 +256,57 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -317,13 +317,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,19 +335,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,7 +353,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,73 +365,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,7 +389,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,19 +437,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,13 +497,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,39 +508,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -558,8 +525,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,6 +551,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -608,151 +599,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1889,16 +1889,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>667385</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>509905</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>250190</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>113030</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>208915</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1906,8 +1906,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3362960" y="487680"/>
-        <a:ext cx="7326630" cy="4425950"/>
+        <a:off x="2157730" y="9525"/>
+        <a:ext cx="9176385" cy="6115050"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1920,15 +1920,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>429260</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>200660</xdr:rowOff>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>121285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>438785</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>172085</xdr:rowOff>
+      <xdr:colOff>794385</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>83185</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1937,8 +1937,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3915410" y="1400175"/>
-          <a:ext cx="1933575" cy="972185"/>
+          <a:off x="3501390" y="921385"/>
+          <a:ext cx="2703195" cy="1762125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2074,7 +2074,7 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1400">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -2082,7 +2082,7 @@
             </a:rPr>
             <a:t>orange: QM - 385 (ev)</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
+          <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
               <a:schemeClr val="accent4"/>
             </a:solidFill>
@@ -2092,7 +2092,7 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1400">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -2106,7 +2106,7 @@
             </a:rPr>
             <a:t>blue:     Edisp (ev)</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
+          <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
@@ -2139,8 +2139,8 @@
     </cdr:to>
     <cdr:sp>
       <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="Text Box 1"/>
-        <cdr:cNvSpPr txBox="1"/>
+        <cdr:cNvPr id="2" name="Rectangle 1"/>
+        <cdr:cNvSpPr/>
       </cdr:nvSpPr>
       <cdr:spPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -2170,8 +2170,8 @@
     </cdr:to>
     <cdr:sp>
       <cdr:nvSpPr>
-        <cdr:cNvPr id="4" name="Text Box 3"/>
-        <cdr:cNvSpPr txBox="1"/>
+        <cdr:cNvPr id="3" name="Rectangle 2"/>
+        <cdr:cNvSpPr/>
       </cdr:nvSpPr>
       <cdr:spPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -2937,8 +2937,8 @@
   <sheetPr/>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>

</xml_diff>